<commit_message>
update: atom snippets.cson;learnling logs;etc.
</commit_message>
<xml_diff>
--- a/工作周报.xlsx
+++ b/工作周报.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11670" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Done" sheetId="1" r:id="rId1"/>
@@ -986,7 +986,8 @@
   <si>
     <t>1.有课后台:update: a)创建班级时，选择助教
                    b)班级列表，搜索不到该手机号时的提示
-                   c) 创建课程改为竖屏;其他小改动</t>
+                   c) 创建课程改为竖屏;其他小改动
+2.有课后台:add:财务管理 a) 充值</t>
   </si>
 </sst>
 </file>
@@ -994,30 +995,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1032,9 +1018,48 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1047,6 +1072,53 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1067,70 +1139,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1139,14 +1148,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1183,7 +1184,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1195,18 +1220,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1219,6 +1232,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1231,7 +1304,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1243,127 +1352,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1374,6 +1375,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1388,6 +1428,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1410,67 +1470,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1482,10 +1483,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1494,133 +1495,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
update: sync-settings backup;learn note;
</commit_message>
<xml_diff>
--- a/工作周报.xlsx
+++ b/工作周报.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="180">
   <si>
     <t>2018/7/17
 ~2018/7/20</t>
@@ -1004,8 +1004,16 @@
 ~2020/4/17</t>
   </si>
   <si>
-    <t>1.有课后台:财务管理：fix: 1.分页bug；余额每个页面重新查询一次；: 导出账单标题中文,order_id不显示等等。
+    <t>1.有课后台:财务管理：fix: 1.分页bug；余额每个页面重新查询一次；: 导出账单标题中文,order_id不显示等等。fix: excel中数字列不能求和的bug
                     update: 1.外观样式调整等</t>
+  </si>
+  <si>
+    <t>2020/4/20
+~2020/4/24</t>
+  </si>
+  <si>
+    <t>1.有课后台:财务管理：update: 1.查询条件保存上次的,回退时恢复
+2.海豚线索:直播管理：1.add: 创建直播间增加video_id字段</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1021,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1034,10 +1042,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1048,39 +1065,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1094,24 +1081,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1126,32 +1120,38 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1165,7 +1165,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1202,7 +1210,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1214,13 +1252,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1232,157 +1384,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1393,36 +1401,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1444,26 +1422,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1483,6 +1443,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1493,6 +1468,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1501,145 +1509,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2394,10 +2402,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -3012,6 +3020,14 @@
       </c>
       <c r="B76" s="2" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="77" ht="201" customHeight="1" spans="1:2">
+      <c r="A77" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- [ ] 完善解决方案:convert-term-case; - [ ] 配置atom-clock插件，并备份该插件; - [ ] 更换Atom syntax theme:atom-material-syntax
</commit_message>
<xml_diff>
--- a/工作周报.xlsx
+++ b/工作周报.xlsx
@@ -1012,8 +1012,10 @@
 ~2020/4/24</t>
   </si>
   <si>
-    <t>1.有课后台:财务管理：update: 1.查询条件保存上次的,回退时恢复
-2.海豚线索:直播管理：1.add: 创建直播间增加video_id字段</t>
+    <t xml:space="preserve">1.有课后台:财务管理：update: 1.查询条件保存上次的,回退时恢复
+2.海豚线索:直播管理：a)add: 创建直播间增加可选视频列表选项
+                    b)add: 上传伪直播的视频
+</t>
   </si>
 </sst>
 </file>

</xml_diff>